<commit_message>
Export to Excel Final
</commit_message>
<xml_diff>
--- a/hii.xlsx
+++ b/hii.xlsx
@@ -22,16 +22,16 @@
     <t>Dust Level</t>
   </si>
   <si>
-    <t>17:59:22</t>
-  </si>
-  <si>
-    <t>72.69232558533903</t>
-  </si>
-  <si>
-    <t>57.11054674244281</t>
-  </si>
-  <si>
-    <t>94.55549292934012</t>
+    <t>20:5:27</t>
+  </si>
+  <si>
+    <t>22.804822310888497</t>
+  </si>
+  <si>
+    <t>0.585938</t>
+  </si>
+  <si>
+    <t>4.987632144992207</t>
   </si>
 </sst>
 </file>
@@ -387,10 +387,10 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
         <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:2">

</xml_diff>